<commit_message>
Add requiremenets, change menu
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -692,155 +692,151 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1">
-        <v>5</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="3">
-        <v>7</v>
-      </c>
-      <c r="D1" s="4">
-        <v>2</v>
-      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
+      <c r="F1" s="3">
+        <v>6</v>
+      </c>
       <c r="G1" s="4"/>
       <c r="H1" s="2"/>
       <c r="I1" s="3">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J1" s="5"/>
     </row>
     <row r="2">
       <c r="A2" s="6">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
+      <c r="D2" s="9">
+        <v>7</v>
+      </c>
       <c r="E2" s="7">
-        <v>9</v>
-      </c>
-      <c r="F2" s="8">
-        <v>6</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I2" s="8"/>
     </row>
     <row r="3">
-      <c r="A3" s="10"/>
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
+      <c r="C3" s="12">
+        <v>6</v>
+      </c>
       <c r="D3" s="13"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="12">
-        <v>8</v>
-      </c>
+      <c r="F3" s="12"/>
       <c r="G3" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="12">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4"/>
-      <c r="B4" s="14">
-        <v>1</v>
-      </c>
+      <c r="B4" s="14"/>
       <c r="C4" s="15"/>
       <c r="D4" s="1"/>
       <c r="E4" s="14"/>
       <c r="F4" s="15"/>
-      <c r="G4" s="1">
-        <v>3</v>
-      </c>
+      <c r="G4" s="1"/>
       <c r="H4" s="14"/>
       <c r="I4" s="15"/>
     </row>
     <row r="5">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="8">
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="7">
+        <v>8</v>
+      </c>
+      <c r="F5" s="8">
+        <v>2</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="7">
         <v>5</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="8">
-        <v>4</v>
-      </c>
+      <c r="I5" s="8"/>
     </row>
     <row r="6">
-      <c r="A6" s="10">
-        <v>2</v>
-      </c>
+      <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
-      <c r="E6" s="11">
-        <v>1</v>
-      </c>
+      <c r="E6" s="11"/>
       <c r="F6" s="12"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="11"/>
+      <c r="H6" s="11">
+        <v>8</v>
+      </c>
       <c r="I6" s="12">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4">
-        <v>1</v>
-      </c>
-      <c r="B7" s="14">
-        <v>9</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B7" s="14"/>
       <c r="C7" s="15"/>
       <c r="D7" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="15"/>
       <c r="G7" s="1"/>
       <c r="H7" s="14"/>
       <c r="I7" s="15">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8">
-        <v>2</v>
-      </c>
+      <c r="B8" s="7">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8"/>
       <c r="D8" s="9"/>
       <c r="E8" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
+      <c r="G8" s="9">
+        <v>8</v>
+      </c>
       <c r="H8" s="7"/>
       <c r="I8" s="8"/>
     </row>
     <row r="9">
       <c r="A9" s="10">
-        <v>6</v>
-      </c>
-      <c r="B9" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="B9" s="11">
+        <v>2</v>
+      </c>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="11">
-        <v>7</v>
-      </c>
-      <c r="F9" s="12"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12">
+        <v>9</v>
+      </c>
       <c r="G9" s="13">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="12"/>

</xml_diff>